<commit_message>
add ajuste product list
</commit_message>
<xml_diff>
--- a/DATA/ProductsList.xlsx
+++ b/DATA/ProductsList.xlsx
@@ -665,7 +665,7 @@
   </sheetPr>
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="36" zoomScaleNormal="36" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -684,8 +684,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16383" min="16383" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>